<commit_message>
Modify lexicon to add new reserved words, $ and #
</commit_message>
<xml_diff>
--- a/src/resources/matriz_lexico.xlsx
+++ b/src/resources/matriz_lexico.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguir\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguir\Desktop\compi\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC085583-A649-4924-B296-BD37A54421BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96E82AE-C682-469D-89C9-12D75C7EF1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{58E676C6-F54D-4C23-987C-94EFFD95D95D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>+</t>
   </si>
@@ -142,6 +142,12 @@
   <si>
     <t>0-9</t>
   </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
 </sst>
 </file>
 
@@ -170,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +212,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -222,7 +234,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -249,6 +261,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -590,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51591C8B-2DFC-4221-BCD0-682DFBDFEC23}">
   <dimension ref="A1:CD100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+    <sheetView tabSelected="1" topLeftCell="V52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AL70" sqref="AL70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,8 +718,12 @@
       <c r="AJ1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
+      <c r="AK1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -859,8 +878,12 @@
       <c r="AJ2" s="3">
         <v>500</v>
       </c>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
+      <c r="AK2" s="10">
+        <v>65</v>
+      </c>
+      <c r="AL2" s="10">
+        <v>67</v>
+      </c>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1015,8 +1038,12 @@
       <c r="AJ3" s="4">
         <v>-1</v>
       </c>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
+      <c r="AK3" s="4">
+        <v>-1</v>
+      </c>
+      <c r="AL3" s="4">
+        <v>-1</v>
+      </c>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
@@ -1171,8 +1198,12 @@
       <c r="AJ4" s="8">
         <v>-4</v>
       </c>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
+      <c r="AK4" s="8">
+        <v>-4</v>
+      </c>
+      <c r="AL4" s="8">
+        <v>-4</v>
+      </c>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
@@ -1327,8 +1358,12 @@
       <c r="AJ5" s="8">
         <v>-7</v>
       </c>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
+      <c r="AK5" s="8">
+        <v>-7</v>
+      </c>
+      <c r="AL5" s="8">
+        <v>-7</v>
+      </c>
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
@@ -1483,8 +1518,12 @@
       <c r="AJ6" s="8">
         <v>-8</v>
       </c>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
+      <c r="AK6" s="8">
+        <v>-8</v>
+      </c>
+      <c r="AL6" s="8">
+        <v>-8</v>
+      </c>
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
@@ -1639,8 +1678,12 @@
       <c r="AJ7" s="8">
         <v>-10</v>
       </c>
-      <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
+      <c r="AK7" s="8">
+        <v>-10</v>
+      </c>
+      <c r="AL7" s="8">
+        <v>-10</v>
+      </c>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
@@ -1795,8 +1838,12 @@
       <c r="AJ8" s="8">
         <v>-13</v>
       </c>
-      <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
+      <c r="AK8" s="8">
+        <v>-13</v>
+      </c>
+      <c r="AL8" s="8">
+        <v>-13</v>
+      </c>
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
@@ -1951,8 +1998,12 @@
       <c r="AJ9" s="8">
         <v>-15</v>
       </c>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
+      <c r="AK9" s="8">
+        <v>-15</v>
+      </c>
+      <c r="AL9" s="8">
+        <v>-15</v>
+      </c>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
@@ -2107,8 +2158,12 @@
       <c r="AJ10" s="8">
         <v>-16</v>
       </c>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
+      <c r="AK10" s="8">
+        <v>-16</v>
+      </c>
+      <c r="AL10" s="8">
+        <v>-16</v>
+      </c>
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
@@ -2263,8 +2318,12 @@
       <c r="AJ11" s="8">
         <v>-17</v>
       </c>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
+      <c r="AK11" s="8">
+        <v>-17</v>
+      </c>
+      <c r="AL11" s="8">
+        <v>-17</v>
+      </c>
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
@@ -2419,8 +2478,12 @@
       <c r="AJ12" s="8">
         <v>-18</v>
       </c>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
+      <c r="AK12" s="8">
+        <v>-18</v>
+      </c>
+      <c r="AL12" s="8">
+        <v>-18</v>
+      </c>
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
@@ -2575,8 +2638,12 @@
       <c r="AJ13" s="8">
         <v>-19</v>
       </c>
-      <c r="AK13" s="1"/>
-      <c r="AL13" s="1"/>
+      <c r="AK13" s="8">
+        <v>-19</v>
+      </c>
+      <c r="AL13" s="8">
+        <v>-19</v>
+      </c>
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
@@ -2731,8 +2798,12 @@
       <c r="AJ14" s="8">
         <v>-22</v>
       </c>
-      <c r="AK14" s="1"/>
-      <c r="AL14" s="1"/>
+      <c r="AK14" s="8">
+        <v>-22</v>
+      </c>
+      <c r="AL14" s="8">
+        <v>-22</v>
+      </c>
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
@@ -2887,8 +2958,12 @@
       <c r="AJ15" s="8">
         <v>-25</v>
       </c>
-      <c r="AK15" s="1"/>
-      <c r="AL15" s="1"/>
+      <c r="AK15" s="8">
+        <v>-25</v>
+      </c>
+      <c r="AL15" s="8">
+        <v>-25</v>
+      </c>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
@@ -3043,8 +3118,12 @@
       <c r="AJ16" s="8">
         <v>-27</v>
       </c>
-      <c r="AK16" s="1"/>
-      <c r="AL16" s="1"/>
+      <c r="AK16" s="8">
+        <v>-27</v>
+      </c>
+      <c r="AL16" s="8">
+        <v>-27</v>
+      </c>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
@@ -3199,8 +3278,12 @@
       <c r="AJ17" s="8">
         <v>-32</v>
       </c>
-      <c r="AK17" s="1"/>
-      <c r="AL17" s="1"/>
+      <c r="AK17" s="8">
+        <v>-32</v>
+      </c>
+      <c r="AL17" s="8">
+        <v>-32</v>
+      </c>
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
@@ -3355,8 +3438,12 @@
       <c r="AJ18" s="8">
         <v>-38</v>
       </c>
-      <c r="AK18" s="1"/>
-      <c r="AL18" s="1"/>
+      <c r="AK18" s="8">
+        <v>-38</v>
+      </c>
+      <c r="AL18" s="8">
+        <v>-38</v>
+      </c>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
@@ -3511,8 +3598,12 @@
       <c r="AJ19" s="8">
         <v>-42</v>
       </c>
-      <c r="AK19" s="1"/>
-      <c r="AL19" s="1"/>
+      <c r="AK19" s="8">
+        <v>-42</v>
+      </c>
+      <c r="AL19" s="8">
+        <v>-42</v>
+      </c>
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
@@ -3667,8 +3758,12 @@
       <c r="AJ20" s="8">
         <v>-45</v>
       </c>
-      <c r="AK20" s="1"/>
-      <c r="AL20" s="1"/>
+      <c r="AK20" s="8">
+        <v>-45</v>
+      </c>
+      <c r="AL20" s="8">
+        <v>-45</v>
+      </c>
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
@@ -3823,8 +3918,12 @@
       <c r="AJ21" s="8">
         <v>-46</v>
       </c>
-      <c r="AK21" s="1"/>
-      <c r="AL21" s="1"/>
+      <c r="AK21" s="8">
+        <v>-46</v>
+      </c>
+      <c r="AL21" s="8">
+        <v>-46</v>
+      </c>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
@@ -3979,8 +4078,12 @@
       <c r="AJ22" s="8">
         <v>-47</v>
       </c>
-      <c r="AK22" s="1"/>
-      <c r="AL22" s="1"/>
+      <c r="AK22" s="8">
+        <v>-47</v>
+      </c>
+      <c r="AL22" s="8">
+        <v>-47</v>
+      </c>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
@@ -4135,8 +4238,12 @@
       <c r="AJ23" s="8">
         <v>-48</v>
       </c>
-      <c r="AK23" s="1"/>
-      <c r="AL23" s="1"/>
+      <c r="AK23" s="8">
+        <v>-48</v>
+      </c>
+      <c r="AL23" s="8">
+        <v>-48</v>
+      </c>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
@@ -4291,8 +4398,12 @@
       <c r="AJ24" s="8">
         <v>-49</v>
       </c>
-      <c r="AK24" s="1"/>
-      <c r="AL24" s="1"/>
+      <c r="AK24" s="8">
+        <v>-49</v>
+      </c>
+      <c r="AL24" s="8">
+        <v>-49</v>
+      </c>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
@@ -4447,8 +4558,12 @@
       <c r="AJ25" s="8">
         <v>-50</v>
       </c>
-      <c r="AK25" s="1"/>
-      <c r="AL25" s="1"/>
+      <c r="AK25" s="8">
+        <v>-50</v>
+      </c>
+      <c r="AL25" s="8">
+        <v>-50</v>
+      </c>
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
@@ -4603,8 +4718,12 @@
       <c r="AJ26" s="8">
         <v>-51</v>
       </c>
-      <c r="AK26" s="1"/>
-      <c r="AL26" s="1"/>
+      <c r="AK26" s="8">
+        <v>-51</v>
+      </c>
+      <c r="AL26" s="8">
+        <v>-51</v>
+      </c>
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
@@ -4759,8 +4878,12 @@
       <c r="AJ27" s="2">
         <v>25</v>
       </c>
-      <c r="AK27" s="1"/>
-      <c r="AL27" s="1"/>
+      <c r="AK27" s="2">
+        <v>25</v>
+      </c>
+      <c r="AL27" s="2">
+        <v>25</v>
+      </c>
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
@@ -4915,8 +5038,12 @@
       <c r="AJ28" s="2">
         <v>26</v>
       </c>
-      <c r="AK28" s="1"/>
-      <c r="AL28" s="1"/>
+      <c r="AK28" s="2">
+        <v>26</v>
+      </c>
+      <c r="AL28" s="2">
+        <v>26</v>
+      </c>
       <c r="AM28" s="1"/>
       <c r="AN28" s="1"/>
       <c r="AO28" s="1"/>
@@ -5071,8 +5198,12 @@
       <c r="AJ29" s="8">
         <v>-54</v>
       </c>
-      <c r="AK29" s="1"/>
-      <c r="AL29" s="1"/>
+      <c r="AK29" s="8">
+        <v>-54</v>
+      </c>
+      <c r="AL29" s="8">
+        <v>-54</v>
+      </c>
       <c r="AM29" s="1"/>
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
@@ -5227,8 +5358,12 @@
       <c r="AJ30" s="8">
         <v>-59</v>
       </c>
-      <c r="AK30" s="1"/>
-      <c r="AL30" s="1"/>
+      <c r="AK30" s="8">
+        <v>-59</v>
+      </c>
+      <c r="AL30" s="8">
+        <v>-59</v>
+      </c>
       <c r="AM30" s="1"/>
       <c r="AN30" s="1"/>
       <c r="AO30" s="1"/>
@@ -5383,8 +5518,12 @@
       <c r="AJ31" s="4">
         <v>-2</v>
       </c>
-      <c r="AK31" s="1"/>
-      <c r="AL31" s="1"/>
+      <c r="AK31" s="4">
+        <v>-2</v>
+      </c>
+      <c r="AL31" s="4">
+        <v>-2</v>
+      </c>
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
@@ -5539,8 +5678,12 @@
       <c r="AJ32" s="4">
         <v>-3</v>
       </c>
-      <c r="AK32" s="1"/>
-      <c r="AL32" s="1"/>
+      <c r="AK32" s="4">
+        <v>-3</v>
+      </c>
+      <c r="AL32" s="4">
+        <v>-3</v>
+      </c>
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
       <c r="AO32" s="1"/>
@@ -5695,8 +5838,12 @@
       <c r="AJ33" s="8">
         <v>-5</v>
       </c>
-      <c r="AK33" s="1"/>
-      <c r="AL33" s="1"/>
+      <c r="AK33" s="8">
+        <v>-5</v>
+      </c>
+      <c r="AL33" s="8">
+        <v>-5</v>
+      </c>
       <c r="AM33" s="1"/>
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
@@ -5851,8 +5998,12 @@
       <c r="AJ34" s="8">
         <v>-6</v>
       </c>
-      <c r="AK34" s="1"/>
-      <c r="AL34" s="1"/>
+      <c r="AK34" s="8">
+        <v>-6</v>
+      </c>
+      <c r="AL34" s="8">
+        <v>-6</v>
+      </c>
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
       <c r="AO34" s="1"/>
@@ -6007,8 +6158,12 @@
       <c r="AJ35" s="8">
         <v>-9</v>
       </c>
-      <c r="AK35" s="1"/>
-      <c r="AL35" s="1"/>
+      <c r="AK35" s="8">
+        <v>-9</v>
+      </c>
+      <c r="AL35" s="8">
+        <v>-9</v>
+      </c>
       <c r="AM35" s="1"/>
       <c r="AN35" s="1"/>
       <c r="AO35" s="1"/>
@@ -6163,8 +6318,12 @@
       <c r="AJ36" s="8">
         <v>-11</v>
       </c>
-      <c r="AK36" s="1"/>
-      <c r="AL36" s="1"/>
+      <c r="AK36" s="8">
+        <v>-11</v>
+      </c>
+      <c r="AL36" s="8">
+        <v>-11</v>
+      </c>
       <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
@@ -6319,8 +6478,12 @@
       <c r="AJ37" s="8">
         <v>-12</v>
       </c>
-      <c r="AK37" s="1"/>
-      <c r="AL37" s="1"/>
+      <c r="AK37" s="8">
+        <v>-12</v>
+      </c>
+      <c r="AL37" s="8">
+        <v>-12</v>
+      </c>
       <c r="AM37" s="1"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
@@ -6475,8 +6638,12 @@
       <c r="AJ38" s="8">
         <v>-14</v>
       </c>
-      <c r="AK38" s="1"/>
-      <c r="AL38" s="1"/>
+      <c r="AK38" s="8">
+        <v>-14</v>
+      </c>
+      <c r="AL38" s="8">
+        <v>-14</v>
+      </c>
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
       <c r="AO38" s="1"/>
@@ -6631,8 +6798,12 @@
       <c r="AJ39" s="8">
         <v>-20</v>
       </c>
-      <c r="AK39" s="1"/>
-      <c r="AL39" s="1"/>
+      <c r="AK39" s="8">
+        <v>-20</v>
+      </c>
+      <c r="AL39" s="8">
+        <v>-20</v>
+      </c>
       <c r="AM39" s="1"/>
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
@@ -6787,8 +6958,12 @@
       <c r="AJ40" s="8">
         <v>-21</v>
       </c>
-      <c r="AK40" s="1"/>
-      <c r="AL40" s="1"/>
+      <c r="AK40" s="8">
+        <v>-21</v>
+      </c>
+      <c r="AL40" s="8">
+        <v>-21</v>
+      </c>
       <c r="AM40" s="1"/>
       <c r="AN40" s="1"/>
       <c r="AO40" s="1"/>
@@ -6943,8 +7118,12 @@
       <c r="AJ41" s="8">
         <v>-23</v>
       </c>
-      <c r="AK41" s="1"/>
-      <c r="AL41" s="1"/>
+      <c r="AK41" s="8">
+        <v>-23</v>
+      </c>
+      <c r="AL41" s="8">
+        <v>-23</v>
+      </c>
       <c r="AM41" s="1"/>
       <c r="AN41" s="1"/>
       <c r="AO41" s="1"/>
@@ -7099,8 +7278,12 @@
       <c r="AJ42" s="2">
         <v>40</v>
       </c>
-      <c r="AK42" s="1"/>
-      <c r="AL42" s="1"/>
+      <c r="AK42" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL42" s="2">
+        <v>40</v>
+      </c>
       <c r="AM42" s="1"/>
       <c r="AN42" s="1"/>
       <c r="AO42" s="1"/>
@@ -7255,8 +7438,12 @@
       <c r="AJ43" s="2">
         <v>41</v>
       </c>
-      <c r="AK43" s="1"/>
-      <c r="AL43" s="1"/>
+      <c r="AK43" s="2">
+        <v>41</v>
+      </c>
+      <c r="AL43" s="2">
+        <v>41</v>
+      </c>
       <c r="AM43" s="1"/>
       <c r="AN43" s="1"/>
       <c r="AO43" s="1"/>
@@ -7411,8 +7598,12 @@
       <c r="AJ44" s="8">
         <v>-26</v>
       </c>
-      <c r="AK44" s="1"/>
-      <c r="AL44" s="1"/>
+      <c r="AK44" s="8">
+        <v>-26</v>
+      </c>
+      <c r="AL44" s="8">
+        <v>-26</v>
+      </c>
       <c r="AM44" s="1"/>
       <c r="AN44" s="1"/>
       <c r="AO44" s="1"/>
@@ -7567,8 +7758,12 @@
       <c r="AJ45" s="8">
         <v>-28</v>
       </c>
-      <c r="AK45" s="1"/>
-      <c r="AL45" s="1"/>
+      <c r="AK45" s="8">
+        <v>-28</v>
+      </c>
+      <c r="AL45" s="8">
+        <v>-28</v>
+      </c>
       <c r="AM45" s="1"/>
       <c r="AN45" s="1"/>
       <c r="AO45" s="1"/>
@@ -7723,8 +7918,12 @@
       <c r="AJ46" s="8">
         <v>-29</v>
       </c>
-      <c r="AK46" s="1"/>
-      <c r="AL46" s="1"/>
+      <c r="AK46" s="8">
+        <v>-29</v>
+      </c>
+      <c r="AL46" s="8">
+        <v>-29</v>
+      </c>
       <c r="AM46" s="1"/>
       <c r="AN46" s="1"/>
       <c r="AO46" s="1"/>
@@ -7879,8 +8078,12 @@
       <c r="AJ47" s="8">
         <v>-30</v>
       </c>
-      <c r="AK47" s="1"/>
-      <c r="AL47" s="1"/>
+      <c r="AK47" s="8">
+        <v>-30</v>
+      </c>
+      <c r="AL47" s="8">
+        <v>-30</v>
+      </c>
       <c r="AM47" s="1"/>
       <c r="AN47" s="1"/>
       <c r="AO47" s="1"/>
@@ -8035,8 +8238,12 @@
       <c r="AJ48" s="8">
         <v>-31</v>
       </c>
-      <c r="AK48" s="1"/>
-      <c r="AL48" s="1"/>
+      <c r="AK48" s="8">
+        <v>-31</v>
+      </c>
+      <c r="AL48" s="8">
+        <v>-31</v>
+      </c>
       <c r="AM48" s="1"/>
       <c r="AN48" s="1"/>
       <c r="AO48" s="1"/>
@@ -8191,8 +8398,12 @@
       <c r="AJ49" s="8">
         <v>-33</v>
       </c>
-      <c r="AK49" s="1"/>
-      <c r="AL49" s="1"/>
+      <c r="AK49" s="8">
+        <v>-33</v>
+      </c>
+      <c r="AL49" s="8">
+        <v>-33</v>
+      </c>
       <c r="AM49" s="1"/>
       <c r="AN49" s="1"/>
       <c r="AO49" s="1"/>
@@ -8347,8 +8558,12 @@
       <c r="AJ50" s="8">
         <v>-34</v>
       </c>
-      <c r="AK50" s="1"/>
-      <c r="AL50" s="1"/>
+      <c r="AK50" s="8">
+        <v>-34</v>
+      </c>
+      <c r="AL50" s="8">
+        <v>-34</v>
+      </c>
       <c r="AM50" s="1"/>
       <c r="AN50" s="1"/>
       <c r="AO50" s="1"/>
@@ -8503,8 +8718,12 @@
       <c r="AJ51" s="8">
         <v>-35</v>
       </c>
-      <c r="AK51" s="1"/>
-      <c r="AL51" s="1"/>
+      <c r="AK51" s="8">
+        <v>-35</v>
+      </c>
+      <c r="AL51" s="8">
+        <v>-35</v>
+      </c>
       <c r="AM51" s="1"/>
       <c r="AN51" s="1"/>
       <c r="AO51" s="1"/>
@@ -8659,8 +8878,12 @@
       <c r="AJ52" s="8">
         <v>-36</v>
       </c>
-      <c r="AK52" s="1"/>
-      <c r="AL52" s="1"/>
+      <c r="AK52" s="8">
+        <v>-36</v>
+      </c>
+      <c r="AL52" s="8">
+        <v>-36</v>
+      </c>
       <c r="AM52" s="1"/>
       <c r="AN52" s="1"/>
       <c r="AO52" s="1"/>
@@ -8815,8 +9038,12 @@
       <c r="AJ53" s="8">
         <v>-37</v>
       </c>
-      <c r="AK53" s="1"/>
-      <c r="AL53" s="1"/>
+      <c r="AK53" s="8">
+        <v>-37</v>
+      </c>
+      <c r="AL53" s="8">
+        <v>-37</v>
+      </c>
       <c r="AM53" s="1"/>
       <c r="AN53" s="1"/>
       <c r="AO53" s="1"/>
@@ -8971,8 +9198,12 @@
       <c r="AJ54" s="8">
         <v>-39</v>
       </c>
-      <c r="AK54" s="1"/>
-      <c r="AL54" s="1"/>
+      <c r="AK54" s="8">
+        <v>-39</v>
+      </c>
+      <c r="AL54" s="8">
+        <v>-39</v>
+      </c>
       <c r="AM54" s="1"/>
       <c r="AN54" s="1"/>
       <c r="AO54" s="1"/>
@@ -9127,8 +9358,12 @@
       <c r="AJ55" s="8">
         <v>-40</v>
       </c>
-      <c r="AK55" s="1"/>
-      <c r="AL55" s="1"/>
+      <c r="AK55" s="8">
+        <v>-40</v>
+      </c>
+      <c r="AL55" s="8">
+        <v>-40</v>
+      </c>
       <c r="AM55" s="1"/>
       <c r="AN55" s="1"/>
       <c r="AO55" s="1"/>
@@ -9283,8 +9518,12 @@
       <c r="AJ56" s="8">
         <v>-41</v>
       </c>
-      <c r="AK56" s="1"/>
-      <c r="AL56" s="1"/>
+      <c r="AK56" s="8">
+        <v>-41</v>
+      </c>
+      <c r="AL56" s="8">
+        <v>-41</v>
+      </c>
       <c r="AM56" s="1"/>
       <c r="AN56" s="1"/>
       <c r="AO56" s="1"/>
@@ -9439,8 +9678,12 @@
       <c r="AJ57" s="8">
         <v>-43</v>
       </c>
-      <c r="AK57" s="1"/>
-      <c r="AL57" s="1"/>
+      <c r="AK57" s="8">
+        <v>-43</v>
+      </c>
+      <c r="AL57" s="8">
+        <v>-43</v>
+      </c>
       <c r="AM57" s="1"/>
       <c r="AN57" s="1"/>
       <c r="AO57" s="1"/>
@@ -9595,8 +9838,12 @@
       <c r="AJ58" s="8">
         <v>-44</v>
       </c>
-      <c r="AK58" s="1"/>
-      <c r="AL58" s="1"/>
+      <c r="AK58" s="8">
+        <v>-44</v>
+      </c>
+      <c r="AL58" s="8">
+        <v>-44</v>
+      </c>
       <c r="AM58" s="1"/>
       <c r="AN58" s="1"/>
       <c r="AO58" s="1"/>
@@ -9751,8 +9998,12 @@
       <c r="AJ59" s="8">
         <v>-52</v>
       </c>
-      <c r="AK59" s="1"/>
-      <c r="AL59" s="1"/>
+      <c r="AK59" s="8">
+        <v>-52</v>
+      </c>
+      <c r="AL59" s="8">
+        <v>-52</v>
+      </c>
       <c r="AM59" s="1"/>
       <c r="AN59" s="1"/>
       <c r="AO59" s="1"/>
@@ -9907,8 +10158,12 @@
       <c r="AJ60" s="8">
         <v>-53</v>
       </c>
-      <c r="AK60" s="1"/>
-      <c r="AL60" s="1"/>
+      <c r="AK60" s="8">
+        <v>-53</v>
+      </c>
+      <c r="AL60" s="8">
+        <v>-53</v>
+      </c>
       <c r="AM60" s="1"/>
       <c r="AN60" s="1"/>
       <c r="AO60" s="1"/>
@@ -10063,8 +10318,12 @@
       <c r="AJ61" s="3">
         <v>503</v>
       </c>
-      <c r="AK61" s="1"/>
-      <c r="AL61" s="1"/>
+      <c r="AK61" s="3">
+        <v>503</v>
+      </c>
+      <c r="AL61" s="3">
+        <v>503</v>
+      </c>
       <c r="AM61" s="1"/>
       <c r="AN61" s="1"/>
       <c r="AO61" s="1"/>
@@ -10219,8 +10478,12 @@
       <c r="AJ62" s="8">
         <v>-55</v>
       </c>
-      <c r="AK62" s="1"/>
-      <c r="AL62" s="1"/>
+      <c r="AK62" s="8">
+        <v>-55</v>
+      </c>
+      <c r="AL62" s="8">
+        <v>-55</v>
+      </c>
       <c r="AM62" s="1"/>
       <c r="AN62" s="1"/>
       <c r="AO62" s="1"/>
@@ -10375,8 +10638,12 @@
       <c r="AJ63" s="3">
         <v>504</v>
       </c>
-      <c r="AK63" s="1"/>
-      <c r="AL63" s="1"/>
+      <c r="AK63" s="3">
+        <v>504</v>
+      </c>
+      <c r="AL63" s="3">
+        <v>504</v>
+      </c>
       <c r="AM63" s="1"/>
       <c r="AN63" s="1"/>
       <c r="AO63" s="1"/>
@@ -10531,8 +10798,12 @@
       <c r="AJ64" s="3">
         <v>505</v>
       </c>
-      <c r="AK64" s="1"/>
-      <c r="AL64" s="1"/>
+      <c r="AK64" s="3">
+        <v>505</v>
+      </c>
+      <c r="AL64" s="3">
+        <v>505</v>
+      </c>
       <c r="AM64" s="1"/>
       <c r="AN64" s="1"/>
       <c r="AO64" s="1"/>
@@ -10670,7 +10941,7 @@
         <v>506</v>
       </c>
       <c r="AE65" s="2">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AF65" s="3">
         <v>506</v>
@@ -10687,8 +10958,12 @@
       <c r="AJ65" s="3">
         <v>506</v>
       </c>
-      <c r="AK65" s="1"/>
-      <c r="AL65" s="1"/>
+      <c r="AK65" s="3">
+        <v>506</v>
+      </c>
+      <c r="AL65" s="3">
+        <v>506</v>
+      </c>
       <c r="AM65" s="1"/>
       <c r="AN65" s="1"/>
       <c r="AO65" s="1"/>
@@ -10843,8 +11118,12 @@
       <c r="AJ66" s="8">
         <v>-56</v>
       </c>
-      <c r="AK66" s="1"/>
-      <c r="AL66" s="1"/>
+      <c r="AK66" s="8">
+        <v>-56</v>
+      </c>
+      <c r="AL66" s="8">
+        <v>-56</v>
+      </c>
       <c r="AM66" s="1"/>
       <c r="AN66" s="1"/>
       <c r="AO66" s="1"/>
@@ -10981,8 +11260,8 @@
       <c r="AD67" s="8">
         <v>-57</v>
       </c>
-      <c r="AE67" s="2">
-        <v>65</v>
+      <c r="AE67" s="8">
+        <v>-57</v>
       </c>
       <c r="AF67" s="8">
         <v>-57</v>
@@ -10999,7 +11278,12 @@
       <c r="AJ67" s="8">
         <v>-57</v>
       </c>
-      <c r="AL67" s="1"/>
+      <c r="AK67" s="8">
+        <v>-57</v>
+      </c>
+      <c r="AL67" s="8">
+        <v>-57</v>
+      </c>
       <c r="AM67" s="1"/>
       <c r="AN67" s="1"/>
       <c r="AO67" s="1"/>
@@ -11137,7 +11421,7 @@
         <v>507</v>
       </c>
       <c r="AE68" s="2">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AF68" s="3">
         <v>507</v>
@@ -11154,8 +11438,12 @@
       <c r="AJ68" s="3">
         <v>507</v>
       </c>
-      <c r="AK68" s="1"/>
-      <c r="AL68" s="1"/>
+      <c r="AK68" s="3">
+        <v>507</v>
+      </c>
+      <c r="AL68" s="3">
+        <v>507</v>
+      </c>
       <c r="AM68" s="1"/>
       <c r="AN68" s="1"/>
       <c r="AO68" s="1"/>
@@ -11292,8 +11580,8 @@
       <c r="AD69" s="8">
         <v>-58</v>
       </c>
-      <c r="AE69" s="2">
-        <v>67</v>
+      <c r="AE69" s="8">
+        <v>-58</v>
       </c>
       <c r="AF69" s="8">
         <v>-58</v>
@@ -11310,8 +11598,12 @@
       <c r="AJ69" s="8">
         <v>-58</v>
       </c>
-      <c r="AK69" s="1"/>
-      <c r="AL69" s="1"/>
+      <c r="AK69" s="8">
+        <v>-58</v>
+      </c>
+      <c r="AL69" s="8">
+        <v>-58</v>
+      </c>
       <c r="AM69" s="1"/>
       <c r="AN69" s="1"/>
       <c r="AO69" s="1"/>
@@ -11362,91 +11654,91 @@
         <v>68</v>
       </c>
       <c r="B70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="C70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="D70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="E70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="F70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="G70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="H70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="I70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="J70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="K70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="L70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="M70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="N70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="O70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="P70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="Q70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="R70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="S70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="T70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="U70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="V70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="W70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="X70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="Y70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="Z70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="AA70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="AB70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="AC70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="AD70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="AE70" s="2">
         <v>68</v>
@@ -11458,16 +11750,20 @@
         <v>68</v>
       </c>
       <c r="AH70" s="8">
-        <v>-60</v>
+        <v>-59</v>
       </c>
       <c r="AI70" s="2">
         <v>68</v>
       </c>
       <c r="AJ70" s="8">
-        <v>-60</v>
-      </c>
-      <c r="AK70" s="1"/>
-      <c r="AL70" s="1"/>
+        <v>-59</v>
+      </c>
+      <c r="AK70" s="8">
+        <v>-59</v>
+      </c>
+      <c r="AL70" s="8">
+        <v>-59</v>
+      </c>
       <c r="AM70" s="1"/>
       <c r="AN70" s="1"/>
       <c r="AO70" s="1"/>
@@ -11622,8 +11918,12 @@
       <c r="AJ71" s="2">
         <v>41</v>
       </c>
-      <c r="AK71" s="1"/>
-      <c r="AL71" s="1"/>
+      <c r="AK71" s="2">
+        <v>41</v>
+      </c>
+      <c r="AL71" s="2">
+        <v>41</v>
+      </c>
       <c r="AM71" s="1"/>
       <c r="AN71" s="1"/>
       <c r="AO71" s="1"/>
@@ -11778,8 +12078,12 @@
       <c r="AJ72" s="8">
         <v>-61</v>
       </c>
-      <c r="AK72" s="1"/>
-      <c r="AL72" s="1"/>
+      <c r="AK72" s="8">
+        <v>-61</v>
+      </c>
+      <c r="AL72" s="8">
+        <v>-61</v>
+      </c>
       <c r="AM72" s="1"/>
       <c r="AN72" s="1"/>
       <c r="AO72" s="1"/>

</xml_diff>